<commit_message>
matlab et exp 31 34
</commit_message>
<xml_diff>
--- a/Experiences/31to34 holes size.xlsx
+++ b/Experiences/31to34 holes size.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>EXP</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>man</t>
+  </si>
+  <si>
+    <t>inlens</t>
+  </si>
+  <si>
+    <t>pres</t>
+  </si>
+  <si>
+    <t>approxg sur 3-4 lignes</t>
   </si>
 </sst>
 </file>
@@ -145,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -274,11 +283,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,18 +337,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,14 +704,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="19" customWidth="1"/>
     <col min="13" max="13" width="14.44140625" customWidth="1"/>
     <col min="14" max="14" width="17.88671875" customWidth="1"/>
     <col min="15" max="21" width="10.88671875" customWidth="1"/>
@@ -706,14 +734,14 @@
       <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -830,6 +858,23 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
+      <c r="E8" s="24">
+        <v>2</v>
+      </c>
+      <c r="F8" s="25">
+        <v>3</v>
+      </c>
+      <c r="G8" s="25">
+        <v>4</v>
+      </c>
+      <c r="H8" s="25">
+        <v>5</v>
+      </c>
+    </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>15</v>
@@ -858,7 +903,7 @@
       <c r="K9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="M9" t="s">
@@ -887,7 +932,7 @@
       <c r="H10">
         <v>18.989999999999998</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="18">
         <v>31</v>
       </c>
       <c r="M10">
@@ -914,7 +959,7 @@
       <c r="J11" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="18"/>
       <c r="M11">
         <v>21</v>
       </c>
@@ -935,29 +980,64 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="L12" s="20"/>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>18</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
-      <c r="L13" s="20"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
-      <c r="L14" s="20"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
         <v>32</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="18">
         <v>32</v>
       </c>
       <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
-      <c r="L16" s="22" t="s">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20" t="s">
         <v>20</v>
       </c>
       <c r="M16">
@@ -979,30 +1059,47 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
-      <c r="L17" s="20"/>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="L17" s="18"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
-      <c r="L18" s="20"/>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
-      <c r="L19" s="20"/>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C20" s="1">
         <v>33</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L20" s="18">
         <v>33</v>
       </c>
       <c r="M20" s="17"/>
     </row>
-    <row r="21" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
-      <c r="L21" s="20" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <v>21.9</v>
+      </c>
+      <c r="G21">
+        <v>27.9</v>
+      </c>
+      <c r="H21">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L21" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M21">
@@ -1024,32 +1121,72 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C22" s="1"/>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>20.5</v>
+      </c>
+      <c r="E22">
+        <v>25.1</v>
+      </c>
+      <c r="F22">
+        <v>26.1</v>
+      </c>
+      <c r="G22">
+        <v>31</v>
+      </c>
+      <c r="H22">
+        <v>35.6</v>
+      </c>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
-      <c r="L23" s="20"/>
-    </row>
-    <row r="24" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="L23" s="18"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
-      <c r="L24" s="20"/>
-    </row>
-    <row r="25" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C25" s="1">
         <v>34</v>
       </c>
-      <c r="L25" s="20">
+      <c r="L25" s="18">
         <v>34</v>
       </c>
       <c r="M25" s="17">
         <v>48.56</v>
       </c>
     </row>
-    <row r="26" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C26" s="1"/>
-      <c r="L26" s="20" t="s">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>5.48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E26">
+        <v>21.9</v>
+      </c>
+      <c r="F26">
+        <v>27.4</v>
+      </c>
+      <c r="G26">
+        <v>33</v>
+      </c>
+      <c r="H26">
+        <v>34</v>
+      </c>
+      <c r="L26" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M26">
@@ -1068,27 +1205,47 @@
         <v>47.6</v>
       </c>
     </row>
-    <row r="27" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C27" s="1"/>
-      <c r="L27" s="20"/>
-    </row>
-    <row r="28" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>26.3</v>
+      </c>
+      <c r="E27">
+        <v>30.6</v>
+      </c>
+      <c r="F27">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="G27">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H27">
+        <v>39</v>
+      </c>
+      <c r="L27" s="18"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="M32" s="1"/>
     </row>

</xml_diff>